<commit_message>
replace template files with better later verion *.md converts
</commit_message>
<xml_diff>
--- a/inputs/demo-partB2/排版示例-信息.xlsx
+++ b/inputs/demo-partB2/排版示例-信息.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="85">
   <si>
     <t>题型</t>
   </si>
@@ -69,25 +69,28 @@
     <t>Trans</t>
   </si>
   <si>
+    <t>The Atlantic</t>
+  </si>
+  <si>
+    <t>The Guardian</t>
+  </si>
+  <si>
+    <t>Scientific American</t>
+  </si>
+  <si>
+    <t>Huffington Post</t>
+  </si>
+  <si>
+    <t>The Christian Science Monitor</t>
+  </si>
+  <si>
+    <t>Womanitely</t>
+  </si>
+  <si>
     <t>Fortune</t>
   </si>
   <si>
-    <t>The Guardian</t>
-  </si>
-  <si>
-    <t>Scientific American</t>
-  </si>
-  <si>
-    <t>Huffington Post</t>
-  </si>
-  <si>
-    <t>The Christian Science Monitor</t>
-  </si>
-  <si>
-    <t>Womanitely</t>
-  </si>
-  <si>
-    <t>2018-4-13</t>
+    <t>2016-6-28</t>
   </si>
   <si>
     <t>2015-07-05</t>
@@ -111,16 +114,28 @@
     <t>S</t>
   </si>
   <si>
-    <t>P</t>
-  </si>
-  <si>
     <t>E</t>
   </si>
   <si>
-    <t>379</t>
-  </si>
-  <si>
-    <t>Sitting Is Bad for Your Health. Standing May Not Be Great Either. So What Should You Do at Work?</t>
+    <t>329</t>
+  </si>
+  <si>
+    <t>405</t>
+  </si>
+  <si>
+    <t>421</t>
+  </si>
+  <si>
+    <t>399</t>
+  </si>
+  <si>
+    <t>398</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Would a Work-Free World Be So Bad?</t>
   </si>
   <si>
     <t>The Olympic legacy: running out of steam</t>
@@ -141,7 +156,7 @@
     <t>Masazo Nonaka, World's Oldest Living Man, Celebrates 113th Birthday</t>
   </si>
   <si>
-    <t>Jamie Ducharme</t>
+    <t>Ilana E. Strauss</t>
   </si>
   <si>
     <t>Olivia Solon</t>
@@ -159,10 +174,13 @@
     <t>RENAE REINTS</t>
   </si>
   <si>
+    <t>Guo Zongyao</t>
+  </si>
+  <si>
     <t>Zhang Shichao</t>
   </si>
   <si>
-    <t>2018-9-1</t>
+    <t>2017-12-11</t>
   </si>
   <si>
     <t>2017-10-13</t>
@@ -183,7 +201,7 @@
     <t>2018-9-5</t>
   </si>
   <si>
-    <t>http://www.fortunechina.com/life/c/2018-04/22/content_305678.htm</t>
+    <t>https://www.theatlantic.com/business/archive/2016/06/would-a-world-without-work-be-so-bad/488711/</t>
   </si>
   <si>
     <t>https://www.theguardian.com/commentisfree/2015/jul/05/the-guardian-view-on-the-olympic-legacy-running-out-of-steam</t>
@@ -250,9 +268,6 @@
   </si>
   <si>
     <t>prep</t>
-  </si>
-  <si>
-    <t>pron</t>
   </si>
   <si>
     <t>v</t>
@@ -672,25 +687,25 @@
         <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
       </c>
       <c r="E2" t="s">
         <v>33</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="G2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I2" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -701,22 +716,22 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3">
-        <v>405</v>
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="I3" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -727,25 +742,25 @@
         <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
         <v>31</v>
       </c>
-      <c r="E4">
-        <v>421</v>
+      <c r="E4" t="s">
+        <v>35</v>
       </c>
       <c r="F4" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="G4" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="I4" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -756,25 +771,25 @@
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
         <v>32</v>
       </c>
-      <c r="E5">
-        <v>399</v>
+      <c r="E5" t="s">
+        <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="G5" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="I5" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -785,25 +800,25 @@
         <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6">
-        <v>398</v>
+        <v>31</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G6" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="I6" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -814,22 +829,25 @@
         <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7">
-        <v>550</v>
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
       </c>
       <c r="F7" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="G7" t="s">
-        <v>45</v>
+        <v>50</v>
+      </c>
+      <c r="H7" t="s">
+        <v>52</v>
       </c>
       <c r="I7" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -837,28 +855,28 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E8">
         <v>154</v>
       </c>
       <c r="F8" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="G8" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="H8" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="I8" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -885,34 +903,34 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -985,7 +1003,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="B6">
         <v>9</v>
@@ -1022,73 +1040,67 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>8</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
         <v>4</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>6</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
       <c r="I2">
-        <v>4</v>
-      </c>
-      <c r="J2">
         <v>20</v>
       </c>
     </row>

</xml_diff>